<commit_message>
Multiple edits and chart changes
</commit_message>
<xml_diff>
--- a/SUVs and emissions/Car_stats.xlsx
+++ b/SUVs and emissions/Car_stats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Top 10 sold" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="58">
   <si>
     <t xml:space="preserve">Brand</t>
   </si>
@@ -171,16 +171,13 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">Fiesta </t>
-  </si>
-  <si>
     <t xml:space="preserve">Standard</t>
   </si>
   <si>
-    <t xml:space="preserve">Crossover</t>
+    <t xml:space="preserve">Small SUV</t>
   </si>
   <si>
-    <t xml:space="preserve">Small SUV</t>
+    <t xml:space="preserve">Crossover</t>
   </si>
   <si>
     <t xml:space="preserve">Med SUV</t>
@@ -196,9 +193,6 @@
   </si>
   <si>
     <t xml:space="preserve">Ford Fiesta CO2 figures prior to 2008 are calculated as is the 2002 BMW 3 Series CO2 figure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In 2017 the basic Fiesta became a crossover</t>
   </si>
   <si>
     <t xml:space="preserve">The 2008 Ford Kuga only came as a deisel in the basic model, so figures for this are used. Petrol engines were more powerful</t>
@@ -304,10 +298,8 @@
   </sheetPr>
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="O38" activeCellId="0" sqref="O38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K60" activeCellId="0" sqref="K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -978,10 +970,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G269"/>
+  <dimension ref="A1:G267"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B13" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O59" activeCellId="0" sqref="O59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A201" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B244" activeCellId="0" sqref="B244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1014,7 +1006,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>2002</v>
@@ -1029,7 +1021,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1037,7 +1029,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>2003</v>
@@ -1052,7 +1044,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1060,7 +1052,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>2004</v>
@@ -1075,7 +1067,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1083,7 +1075,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2005</v>
@@ -1098,7 +1090,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1106,7 +1098,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>2006</v>
@@ -1121,7 +1113,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1129,7 +1121,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>2007</v>
@@ -1144,7 +1136,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1152,7 +1144,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>2008</v>
@@ -1167,7 +1159,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1175,7 +1167,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>2009</v>
@@ -1190,7 +1182,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1198,7 +1190,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>2010</v>
@@ -1213,7 +1205,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1221,7 +1213,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>2011</v>
@@ -1236,7 +1228,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1244,7 +1236,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>2012</v>
@@ -1259,7 +1251,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1267,7 +1259,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>2013</v>
@@ -1282,7 +1274,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1290,7 +1282,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>2014</v>
@@ -1305,7 +1297,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1313,7 +1305,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>2015</v>
@@ -1328,7 +1320,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1336,7 +1328,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>2016</v>
@@ -1351,7 +1343,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1359,22 +1351,22 @@
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>2017</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>1166</v>
+        <v>1130</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F17" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1382,22 +1374,22 @@
         <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>2018</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>1166</v>
+        <v>1130</v>
       </c>
       <c r="E18" s="1" t="n">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F18" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1405,22 +1397,22 @@
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>2019</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>1166</v>
+        <v>1130</v>
       </c>
       <c r="E19" s="1" t="n">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F19" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1428,22 +1420,22 @@
         <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>2020</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>1166</v>
+        <v>1130</v>
       </c>
       <c r="E20" s="1" t="n">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F20" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1451,22 +1443,22 @@
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>2021</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>1166</v>
+        <v>1130</v>
       </c>
       <c r="E21" s="1" t="n">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F21" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1474,22 +1466,22 @@
         <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>2022</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>1166</v>
+        <v>1130</v>
       </c>
       <c r="E22" s="1" t="n">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F22" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1512,7 +1504,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1535,7 +1527,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1558,7 +1550,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1581,7 +1573,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1604,7 +1596,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1627,7 +1619,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1650,7 +1642,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1673,7 +1665,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1696,7 +1688,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1719,7 +1711,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1742,7 +1734,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1765,7 +1757,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1788,7 +1780,7 @@
         <v>1</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1811,7 +1803,7 @@
         <v>1</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1834,7 +1826,7 @@
         <v>1</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1857,7 +1849,7 @@
         <v>0</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1880,7 +1872,7 @@
         <v>0</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1903,7 +1895,7 @@
         <v>0</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1926,7 +1918,7 @@
         <v>0</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1949,7 +1941,7 @@
         <v>0</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1972,7 +1964,7 @@
         <v>0</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1995,7 +1987,7 @@
         <v>0</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2018,7 +2010,7 @@
         <v>0</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2041,7 +2033,7 @@
         <v>0</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2064,7 +2056,7 @@
         <v>0</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2087,7 +2079,7 @@
         <v>0</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2110,7 +2102,7 @@
         <v>0</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2133,7 +2125,7 @@
         <v>0</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2156,7 +2148,7 @@
         <v>0</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2179,7 +2171,7 @@
         <v>0</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2202,7 +2194,7 @@
         <v>0</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2225,7 +2217,7 @@
         <v>0</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2248,7 +2240,7 @@
         <v>0</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2271,7 +2263,7 @@
         <v>0</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2294,7 +2286,7 @@
         <v>0</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2317,7 +2309,7 @@
         <v>0</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2340,7 +2332,7 @@
         <v>0</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2363,7 +2355,7 @@
         <v>0</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2386,7 +2378,7 @@
         <v>0</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2409,7 +2401,7 @@
         <v>0</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2432,7 +2424,7 @@
         <v>0</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2455,7 +2447,7 @@
         <v>0</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2478,7 +2470,7 @@
         <v>0</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2501,7 +2493,7 @@
         <v>0</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2524,7 +2516,7 @@
         <v>0</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2547,7 +2539,7 @@
         <v>0</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2570,7 +2562,7 @@
         <v>0</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2593,7 +2585,7 @@
         <v>0</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2616,7 +2608,7 @@
         <v>0</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2639,7 +2631,7 @@
         <v>0</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2662,7 +2654,7 @@
         <v>0</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2685,7 +2677,7 @@
         <v>0</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2708,7 +2700,7 @@
         <v>0</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2731,7 +2723,7 @@
         <v>0</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2754,7 +2746,7 @@
         <v>0</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2777,7 +2769,7 @@
         <v>0</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2800,7 +2792,7 @@
         <v>0</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2823,7 +2815,7 @@
         <v>0</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2846,7 +2838,7 @@
         <v>0</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2869,7 +2861,7 @@
         <v>0</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2892,7 +2884,7 @@
         <v>0</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2915,7 +2907,7 @@
         <v>0</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2938,7 +2930,7 @@
         <v>0</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2961,7 +2953,7 @@
         <v>0</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2984,7 +2976,7 @@
         <v>0</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3007,7 +2999,7 @@
         <v>0</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3030,7 +3022,7 @@
         <v>0</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3053,7 +3045,7 @@
         <v>0</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3076,7 +3068,7 @@
         <v>0</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3099,7 +3091,7 @@
         <v>0</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3122,7 +3114,7 @@
         <v>0</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3145,7 +3137,7 @@
         <v>0</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3168,7 +3160,7 @@
         <v>0</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3191,7 +3183,7 @@
         <v>0</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3214,7 +3206,7 @@
         <v>0</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3237,7 +3229,7 @@
         <v>0</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3260,7 +3252,7 @@
         <v>0</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3283,7 +3275,7 @@
         <v>0</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3306,7 +3298,7 @@
         <v>0</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3329,7 +3321,7 @@
         <v>0</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3352,7 +3344,7 @@
         <v>0</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3375,7 +3367,7 @@
         <v>0</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3398,7 +3390,7 @@
         <v>0</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3421,7 +3413,7 @@
         <v>0</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3444,7 +3436,7 @@
         <v>0</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3467,7 +3459,7 @@
         <v>0</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3490,7 +3482,7 @@
         <v>0</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3513,7 +3505,7 @@
         <v>0</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3536,7 +3528,7 @@
         <v>0</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3559,7 +3551,7 @@
         <v>0</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3582,7 +3574,7 @@
         <v>0</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3605,7 +3597,7 @@
         <v>0</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3628,7 +3620,7 @@
         <v>0</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3651,7 +3643,7 @@
         <v>0</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3674,7 +3666,7 @@
         <v>0</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3697,7 +3689,7 @@
         <v>0</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3720,7 +3712,7 @@
         <v>0</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3743,7 +3735,7 @@
         <v>0</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3766,7 +3758,7 @@
         <v>0</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3789,7 +3781,7 @@
         <v>0</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3812,7 +3804,7 @@
         <v>0</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3835,7 +3827,7 @@
         <v>0</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3858,7 +3850,7 @@
         <v>0</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3881,7 +3873,7 @@
         <v>0</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3904,7 +3896,7 @@
         <v>0</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3927,7 +3919,7 @@
         <v>0</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3950,7 +3942,7 @@
         <v>0</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3973,7 +3965,7 @@
         <v>0</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3996,7 +3988,7 @@
         <v>0</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4019,7 +4011,7 @@
         <v>0</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4042,7 +4034,7 @@
         <v>0</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4065,7 +4057,7 @@
         <v>0</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4088,7 +4080,7 @@
         <v>0</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4111,7 +4103,7 @@
         <v>0</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4134,7 +4126,7 @@
         <v>0</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4157,7 +4149,7 @@
         <v>0</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4180,7 +4172,7 @@
         <v>0</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4203,7 +4195,7 @@
         <v>0</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4226,7 +4218,7 @@
         <v>0</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4249,7 +4241,7 @@
         <v>0</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4272,7 +4264,7 @@
         <v>0</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4295,7 +4287,7 @@
         <v>0</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4318,7 +4310,7 @@
         <v>0</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4341,7 +4333,7 @@
         <v>0</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4364,7 +4356,7 @@
         <v>0</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4387,7 +4379,7 @@
         <v>0</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4410,7 +4402,7 @@
         <v>0</v>
       </c>
       <c r="G149" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4433,7 +4425,7 @@
         <v>0</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4456,7 +4448,7 @@
         <v>0</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4479,7 +4471,7 @@
         <v>0</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4502,7 +4494,7 @@
         <v>0</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4525,15 +4517,15 @@
         <v>0</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B155" s="1" t="s">
-        <v>12</v>
+      <c r="B155" s="1" t="n">
+        <v>207</v>
       </c>
       <c r="C155" s="1" t="n">
         <v>2009</v>
@@ -4548,15 +4540,15 @@
         <v>0</v>
       </c>
       <c r="G155" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B156" s="1" t="s">
-        <v>12</v>
+      <c r="B156" s="1" t="n">
+        <v>207</v>
       </c>
       <c r="C156" s="1" t="n">
         <v>2010</v>
@@ -4571,7 +4563,7 @@
         <v>0</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4594,7 +4586,7 @@
         <v>0</v>
       </c>
       <c r="G157" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4617,7 +4609,7 @@
         <v>0</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4640,7 +4632,7 @@
         <v>0</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4663,7 +4655,7 @@
         <v>0</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4686,7 +4678,7 @@
         <v>0</v>
       </c>
       <c r="G161" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4709,7 +4701,7 @@
         <v>0</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4732,7 +4724,7 @@
         <v>0</v>
       </c>
       <c r="G163" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4755,7 +4747,7 @@
         <v>0</v>
       </c>
       <c r="G164" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4778,7 +4770,7 @@
         <v>0</v>
       </c>
       <c r="G165" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4801,7 +4793,7 @@
         <v>0</v>
       </c>
       <c r="G166" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4824,7 +4816,7 @@
         <v>0</v>
       </c>
       <c r="G167" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4847,7 +4839,7 @@
         <v>0</v>
       </c>
       <c r="G168" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4870,7 +4862,7 @@
         <v>0</v>
       </c>
       <c r="G169" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4893,7 +4885,7 @@
         <v>0</v>
       </c>
       <c r="G170" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4916,7 +4908,7 @@
         <v>0</v>
       </c>
       <c r="G171" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4939,7 +4931,7 @@
         <v>0</v>
       </c>
       <c r="G172" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4962,7 +4954,7 @@
         <v>0</v>
       </c>
       <c r="G173" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4985,7 +4977,7 @@
         <v>0</v>
       </c>
       <c r="G174" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5008,7 +5000,7 @@
         <v>0</v>
       </c>
       <c r="G175" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5031,7 +5023,7 @@
         <v>0</v>
       </c>
       <c r="G176" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5054,7 +5046,7 @@
         <v>0</v>
       </c>
       <c r="G177" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5077,7 +5069,7 @@
         <v>0</v>
       </c>
       <c r="G178" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5100,7 +5092,7 @@
         <v>0</v>
       </c>
       <c r="G179" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5123,7 +5115,7 @@
         <v>0</v>
       </c>
       <c r="G180" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5146,7 +5138,7 @@
         <v>0</v>
       </c>
       <c r="G181" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5169,7 +5161,7 @@
         <v>0</v>
       </c>
       <c r="G182" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5192,7 +5184,7 @@
         <v>0</v>
       </c>
       <c r="G183" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5215,7 +5207,7 @@
         <v>0</v>
       </c>
       <c r="G184" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5238,7 +5230,7 @@
         <v>0</v>
       </c>
       <c r="G185" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5261,7 +5253,7 @@
         <v>0</v>
       </c>
       <c r="G186" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5652,7 +5644,7 @@
         <v>0</v>
       </c>
       <c r="G203" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5675,7 +5667,7 @@
         <v>0</v>
       </c>
       <c r="G204" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5698,7 +5690,7 @@
         <v>0</v>
       </c>
       <c r="G205" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5721,7 +5713,7 @@
         <v>0</v>
       </c>
       <c r="G206" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5744,7 +5736,7 @@
         <v>0</v>
       </c>
       <c r="G207" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5767,7 +5759,7 @@
         <v>0</v>
       </c>
       <c r="G208" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5790,7 +5782,7 @@
         <v>0</v>
       </c>
       <c r="G209" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5813,7 +5805,7 @@
         <v>0</v>
       </c>
       <c r="G210" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5836,7 +5828,7 @@
         <v>0</v>
       </c>
       <c r="G211" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5859,7 +5851,7 @@
         <v>0</v>
       </c>
       <c r="G212" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5882,7 +5874,7 @@
         <v>0</v>
       </c>
       <c r="G213" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5905,7 +5897,7 @@
         <v>0</v>
       </c>
       <c r="G214" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5928,7 +5920,7 @@
         <v>0</v>
       </c>
       <c r="G215" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5951,15 +5943,15 @@
         <v>0</v>
       </c>
       <c r="G216" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B217" s="1" t="s">
-        <v>23</v>
+      <c r="B217" s="1" t="n">
+        <v>208</v>
       </c>
       <c r="C217" s="1" t="n">
         <v>2013</v>
@@ -5974,21 +5966,30 @@
         <v>0</v>
       </c>
       <c r="G217" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="1" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="C218" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="D218" s="1" t="n">
+        <v>1205</v>
+      </c>
+      <c r="E218" s="1" t="n">
+        <v>124</v>
       </c>
       <c r="F218" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G218" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5999,7 +6000,7 @@
         <v>26</v>
       </c>
       <c r="C219" s="1" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="D219" s="1" t="n">
         <v>1205</v>
@@ -6022,7 +6023,7 @@
         <v>26</v>
       </c>
       <c r="C220" s="1" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D220" s="1" t="n">
         <v>1205</v>
@@ -6045,7 +6046,7 @@
         <v>26</v>
       </c>
       <c r="C221" s="1" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="D221" s="1" t="n">
         <v>1205</v>
@@ -6062,25 +6063,25 @@
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="1" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C222" s="1" t="n">
-        <v>2022</v>
+        <v>2016</v>
       </c>
       <c r="D222" s="1" t="n">
-        <v>1205</v>
+        <v>1534</v>
       </c>
       <c r="E222" s="1" t="n">
-        <v>124</v>
+        <v>175</v>
       </c>
       <c r="F222" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G222" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6091,7 +6092,7 @@
         <v>28</v>
       </c>
       <c r="C223" s="1" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D223" s="1" t="n">
         <v>1534</v>
@@ -6103,7 +6104,7 @@
         <v>1</v>
       </c>
       <c r="G223" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6114,7 +6115,7 @@
         <v>28</v>
       </c>
       <c r="C224" s="1" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="D224" s="1" t="n">
         <v>1534</v>
@@ -6126,7 +6127,7 @@
         <v>1</v>
       </c>
       <c r="G224" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6137,7 +6138,7 @@
         <v>28</v>
       </c>
       <c r="C225" s="1" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D225" s="1" t="n">
         <v>1534</v>
@@ -6149,7 +6150,7 @@
         <v>1</v>
       </c>
       <c r="G225" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6160,7 +6161,7 @@
         <v>28</v>
       </c>
       <c r="C226" s="1" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="D226" s="1" t="n">
         <v>1534</v>
@@ -6172,7 +6173,7 @@
         <v>1</v>
       </c>
       <c r="G226" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6183,7 +6184,7 @@
         <v>28</v>
       </c>
       <c r="C227" s="1" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D227" s="1" t="n">
         <v>1534</v>
@@ -6195,7 +6196,7 @@
         <v>1</v>
       </c>
       <c r="G227" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6206,42 +6207,42 @@
         <v>28</v>
       </c>
       <c r="C228" s="1" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="D228" s="1" t="n">
-        <v>1534</v>
+        <v>1526</v>
       </c>
       <c r="E228" s="1" t="n">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="F228" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G228" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C229" s="1" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="D229" s="1" t="n">
-        <v>1526</v>
+        <v>1425</v>
       </c>
       <c r="E229" s="1" t="n">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="F229" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G229" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6252,7 +6253,7 @@
         <v>30</v>
       </c>
       <c r="C230" s="1" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="D230" s="1" t="n">
         <v>1425</v>
@@ -6269,25 +6270,25 @@
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C231" s="1" t="n">
-        <v>2022</v>
+        <v>2013</v>
       </c>
       <c r="D231" s="1" t="n">
-        <v>1425</v>
+        <v>1370</v>
       </c>
       <c r="E231" s="1" t="n">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="F231" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G231" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6298,7 +6299,7 @@
         <v>32</v>
       </c>
       <c r="C232" s="1" t="n">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="D232" s="1" t="n">
         <v>1370</v>
@@ -6310,7 +6311,7 @@
         <v>0</v>
       </c>
       <c r="G232" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6321,7 +6322,7 @@
         <v>32</v>
       </c>
       <c r="C233" s="1" t="n">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="D233" s="1" t="n">
         <v>1370</v>
@@ -6333,7 +6334,7 @@
         <v>0</v>
       </c>
       <c r="G233" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6344,7 +6345,7 @@
         <v>32</v>
       </c>
       <c r="C234" s="1" t="n">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="D234" s="1" t="n">
         <v>1370</v>
@@ -6356,7 +6357,7 @@
         <v>0</v>
       </c>
       <c r="G234" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6367,7 +6368,7 @@
         <v>32</v>
       </c>
       <c r="C235" s="1" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D235" s="1" t="n">
         <v>1370</v>
@@ -6379,7 +6380,7 @@
         <v>0</v>
       </c>
       <c r="G235" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6390,19 +6391,19 @@
         <v>32</v>
       </c>
       <c r="C236" s="1" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="D236" s="1" t="n">
-        <v>1370</v>
+        <v>1350</v>
       </c>
       <c r="E236" s="1" t="n">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="F236" s="1" t="n">
         <v>0</v>
       </c>
       <c r="G236" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6413,7 +6414,7 @@
         <v>32</v>
       </c>
       <c r="C237" s="1" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D237" s="1" t="n">
         <v>1350</v>
@@ -6425,7 +6426,7 @@
         <v>0</v>
       </c>
       <c r="G237" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6436,7 +6437,7 @@
         <v>32</v>
       </c>
       <c r="C238" s="1" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="D238" s="1" t="n">
         <v>1350</v>
@@ -6448,7 +6449,7 @@
         <v>0</v>
       </c>
       <c r="G238" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6459,7 +6460,7 @@
         <v>32</v>
       </c>
       <c r="C239" s="1" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D239" s="1" t="n">
         <v>1350</v>
@@ -6471,30 +6472,30 @@
         <v>0</v>
       </c>
       <c r="G239" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C240" s="1" t="n">
-        <v>2021</v>
+        <v>2013</v>
       </c>
       <c r="D240" s="1" t="n">
-        <v>1350</v>
+        <v>1290</v>
       </c>
       <c r="E240" s="1" t="n">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="F240" s="1" t="n">
         <v>0</v>
       </c>
       <c r="G240" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6505,7 +6506,7 @@
         <v>34</v>
       </c>
       <c r="C241" s="1" t="n">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="D241" s="1" t="n">
         <v>1290</v>
@@ -6517,7 +6518,7 @@
         <v>0</v>
       </c>
       <c r="G241" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6528,7 +6529,7 @@
         <v>34</v>
       </c>
       <c r="C242" s="1" t="n">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="D242" s="1" t="n">
         <v>1290</v>
@@ -6540,7 +6541,7 @@
         <v>0</v>
       </c>
       <c r="G242" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6551,53 +6552,53 @@
         <v>34</v>
       </c>
       <c r="C243" s="1" t="n">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="D243" s="1" t="n">
-        <v>1290</v>
+        <v>1260</v>
       </c>
       <c r="E243" s="1" t="n">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="F243" s="1" t="n">
         <v>0</v>
       </c>
       <c r="G243" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B244" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="B244" s="1" t="n">
+        <v>500</v>
       </c>
       <c r="C244" s="1" t="n">
-        <v>2016</v>
+        <v>2007</v>
       </c>
       <c r="D244" s="1" t="n">
-        <v>1260</v>
+        <v>930</v>
       </c>
       <c r="E244" s="1" t="n">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="F244" s="1" t="n">
         <v>0</v>
       </c>
       <c r="G244" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B245" s="1" t="s">
-        <v>36</v>
+      <c r="B245" s="1" t="n">
+        <v>500</v>
       </c>
       <c r="C245" s="1" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="D245" s="1" t="n">
         <v>930</v>
@@ -6609,18 +6610,18 @@
         <v>0</v>
       </c>
       <c r="G245" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B246" s="1" t="s">
-        <v>36</v>
+      <c r="B246" s="1" t="n">
+        <v>500</v>
       </c>
       <c r="C246" s="1" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="D246" s="1" t="n">
         <v>930</v>
@@ -6632,18 +6633,18 @@
         <v>0</v>
       </c>
       <c r="G246" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B247" s="1" t="s">
-        <v>36</v>
+      <c r="B247" s="1" t="n">
+        <v>500</v>
       </c>
       <c r="C247" s="1" t="n">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="D247" s="1" t="n">
         <v>930</v>
@@ -6655,18 +6656,18 @@
         <v>0</v>
       </c>
       <c r="G247" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B248" s="1" t="s">
-        <v>36</v>
+      <c r="B248" s="1" t="n">
+        <v>500</v>
       </c>
       <c r="C248" s="1" t="n">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="D248" s="1" t="n">
         <v>930</v>
@@ -6678,18 +6679,18 @@
         <v>0</v>
       </c>
       <c r="G248" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B249" s="1" t="s">
-        <v>36</v>
+      <c r="B249" s="1" t="n">
+        <v>500</v>
       </c>
       <c r="C249" s="1" t="n">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D249" s="1" t="n">
         <v>930</v>
@@ -6701,18 +6702,18 @@
         <v>0</v>
       </c>
       <c r="G249" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B250" s="1" t="s">
-        <v>36</v>
+      <c r="B250" s="1" t="n">
+        <v>500</v>
       </c>
       <c r="C250" s="1" t="n">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D250" s="1" t="n">
         <v>930</v>
@@ -6724,18 +6725,18 @@
         <v>0</v>
       </c>
       <c r="G250" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B251" s="1" t="s">
-        <v>36</v>
+      <c r="B251" s="1" t="n">
+        <v>500</v>
       </c>
       <c r="C251" s="1" t="n">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="D251" s="1" t="n">
         <v>930</v>
@@ -6747,30 +6748,30 @@
         <v>0</v>
       </c>
       <c r="G251" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="1" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C252" s="1" t="n">
-        <v>2014</v>
+        <v>2010</v>
       </c>
       <c r="D252" s="1" t="n">
-        <v>930</v>
+        <v>1195</v>
       </c>
       <c r="E252" s="1" t="n">
-        <v>92</v>
+        <v>138</v>
       </c>
       <c r="F252" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G252" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6781,7 +6782,7 @@
         <v>37</v>
       </c>
       <c r="C253" s="1" t="n">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="D253" s="1" t="n">
         <v>1195</v>
@@ -6804,7 +6805,7 @@
         <v>37</v>
       </c>
       <c r="C254" s="1" t="n">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D254" s="1" t="n">
         <v>1195</v>
@@ -6827,7 +6828,7 @@
         <v>37</v>
       </c>
       <c r="C255" s="1" t="n">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D255" s="1" t="n">
         <v>1195</v>
@@ -6850,7 +6851,7 @@
         <v>37</v>
       </c>
       <c r="C256" s="1" t="n">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="D256" s="1" t="n">
         <v>1195</v>
@@ -6867,25 +6868,25 @@
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C257" s="1" t="n">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="D257" s="1" t="n">
-        <v>1195</v>
+        <v>1490</v>
       </c>
       <c r="E257" s="1" t="n">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="F257" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G257" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6896,7 +6897,7 @@
         <v>38</v>
       </c>
       <c r="C258" s="1" t="n">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D258" s="1" t="n">
         <v>1490</v>
@@ -6908,7 +6909,7 @@
         <v>1</v>
       </c>
       <c r="G258" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6919,7 +6920,7 @@
         <v>38</v>
       </c>
       <c r="C259" s="1" t="n">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="D259" s="1" t="n">
         <v>1490</v>
@@ -6931,7 +6932,7 @@
         <v>1</v>
       </c>
       <c r="G259" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6942,7 +6943,7 @@
         <v>38</v>
       </c>
       <c r="C260" s="1" t="n">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="D260" s="1" t="n">
         <v>1490</v>
@@ -6954,30 +6955,30 @@
         <v>1</v>
       </c>
       <c r="G260" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="1" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C261" s="1" t="n">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="D261" s="1" t="n">
-        <v>1490</v>
+        <v>1503</v>
       </c>
       <c r="E261" s="1" t="n">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F261" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G261" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6988,7 +6989,7 @@
         <v>40</v>
       </c>
       <c r="C262" s="1" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="D262" s="1" t="n">
         <v>1503</v>
@@ -7000,7 +7001,7 @@
         <v>1</v>
       </c>
       <c r="G262" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7011,7 +7012,7 @@
         <v>40</v>
       </c>
       <c r="C263" s="1" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D263" s="1" t="n">
         <v>1503</v>
@@ -7023,7 +7024,7 @@
         <v>1</v>
       </c>
       <c r="G263" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7034,7 +7035,7 @@
         <v>40</v>
       </c>
       <c r="C264" s="1" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="D264" s="1" t="n">
         <v>1503</v>
@@ -7046,44 +7047,53 @@
         <v>1</v>
       </c>
       <c r="G264" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C265" s="1" t="n">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D265" s="1" t="n">
-        <v>1503</v>
+        <v>940</v>
       </c>
       <c r="E265" s="1" t="n">
-        <v>146</v>
+        <v>92</v>
       </c>
       <c r="F265" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G265" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="1" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="C266" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="D266" s="1" t="n">
+        <v>940</v>
+      </c>
+      <c r="E266" s="1" t="n">
+        <v>92</v>
       </c>
       <c r="F266" s="1" t="n">
         <v>0</v>
       </c>
       <c r="G266" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7094,7 +7104,7 @@
         <v>43</v>
       </c>
       <c r="C267" s="1" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="D267" s="1" t="n">
         <v>940</v>
@@ -7106,53 +7116,7 @@
         <v>0</v>
       </c>
       <c r="G267" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B268" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C268" s="1" t="n">
-        <v>2020</v>
-      </c>
-      <c r="D268" s="1" t="n">
-        <v>940</v>
-      </c>
-      <c r="E268" s="1" t="n">
-        <v>92</v>
-      </c>
-      <c r="F268" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G268" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B269" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C269" s="1" t="n">
-        <v>2021</v>
-      </c>
-      <c r="D269" s="1" t="n">
-        <v>940</v>
-      </c>
-      <c r="E269" s="1" t="n">
-        <v>92</v>
-      </c>
-      <c r="F269" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G269" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -7171,17 +7135,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:B8"/>
+  <dimension ref="A2:E28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
-        <v>54</v>
+      <c r="B2" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7189,7 +7153,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7197,7 +7161,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7205,7 +7169,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7213,16 +7177,85 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>59</v>
-      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D28" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>